<commit_message>
update to app 7 dec
</commit_message>
<xml_diff>
--- a/sloterdijk_master.xlsx
+++ b/sloterdijk_master.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,32 +481,47 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>etrucks</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ebestel</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>opp</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>opp_cat</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Electra_per_m2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>jaarverbruik</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>e-trucks</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>e-bestel</t>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>jaarkilometrage</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>jaarkilometrage_truck</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>jaarkilometrage_bestel</t>
         </is>
       </c>
     </row>
@@ -530,7 +545,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -552,24 +567,33 @@
         </is>
       </c>
       <c r="K2" t="n">
+        <v>70</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
         <v>42100</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>10 000 tot 25 000 m²</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>173.8</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>4800000</v>
       </c>
-      <c r="O2" t="n">
-        <v>3240000</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
+      <c r="Q2" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S2" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="3">
@@ -614,24 +638,33 @@
         </is>
       </c>
       <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
         <v>1421.25</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>47.3</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>67225.125</v>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
+      <c r="Q3" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S3" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="4">
@@ -676,24 +709,33 @@
         </is>
       </c>
       <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>1421.25</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>47.3</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>67225.125</v>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
+      <c r="Q4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="R4" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S4" t="n">
+        <v>20000</v>
       </c>
     </row>
     <row r="5">
@@ -716,10 +758,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -738,24 +780,33 @@
         </is>
       </c>
       <c r="K5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
         <v>2125</v>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>47.3</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>100512.5</v>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
+      <c r="Q5" t="n">
+        <v>22500</v>
+      </c>
+      <c r="R5" t="n">
+        <v>22500</v>
+      </c>
+      <c r="S5" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="6">
@@ -778,10 +829,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -800,24 +851,33 @@
         </is>
       </c>
       <c r="K6" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" t="n">
         <v>1800</v>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>47.3</v>
       </c>
-      <c r="N6" t="n">
+      <c r="P6" t="n">
         <v>41640</v>
       </c>
-      <c r="O6" t="n">
-        <v>288000</v>
-      </c>
-      <c r="P6" t="n">
-        <v>45000</v>
+      <c r="Q6" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R6" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S6" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="7">
@@ -862,24 +922,33 @@
         </is>
       </c>
       <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
         <v>2445</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>178.9</v>
       </c>
-      <c r="N7" t="n">
+      <c r="P7" t="n">
         <v>437410.5</v>
       </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
+      <c r="Q7" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R7" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S7" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="8">
@@ -924,24 +993,33 @@
         </is>
       </c>
       <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
         <v>13742</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>10 000 tot 25 000 m²</t>
         </is>
       </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
         <v>74.09999999999999</v>
       </c>
-      <c r="N8" t="n">
+      <c r="P8" t="n">
         <v>1018282.2</v>
       </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
+      <c r="Q8" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R8" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S8" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="9">
@@ -986,24 +1064,33 @@
         </is>
       </c>
       <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>2550.5</v>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M9" t="n">
+      <c r="O9" t="n">
         <v>70</v>
       </c>
-      <c r="N9" t="n">
+      <c r="P9" t="n">
         <v>178535</v>
       </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
+      <c r="Q9" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R9" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S9" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="10">
@@ -1048,24 +1135,33 @@
         </is>
       </c>
       <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
         <v>2550.5</v>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M10" t="n">
+      <c r="O10" t="n">
         <v>50</v>
       </c>
-      <c r="N10" t="n">
+      <c r="P10" t="n">
         <v>127525</v>
       </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
+      <c r="Q10" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R10" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S10" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="11">
@@ -1110,24 +1206,33 @@
         </is>
       </c>
       <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
         <v>1108.333333333333</v>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M11" t="n">
+      <c r="O11" t="n">
         <v>47.3</v>
       </c>
-      <c r="N11" t="n">
+      <c r="P11" t="n">
         <v>52424.16666666667</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
+      <c r="Q11" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R11" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S11" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="12">
@@ -1172,24 +1277,33 @@
         </is>
       </c>
       <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>1108.333333333333</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>47.3</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>52424.16666666667</v>
       </c>
-      <c r="O12" t="n">
-        <v>180000</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
+      <c r="Q12" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R12" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S12" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="13">
@@ -1234,24 +1348,33 @@
         </is>
       </c>
       <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
         <v>1108.333333333333</v>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>57</v>
       </c>
-      <c r="N13" t="n">
+      <c r="P13" t="n">
         <v>63175.00000000001</v>
       </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
+      <c r="Q13" t="n">
+        <v>15000</v>
+      </c>
+      <c r="R13" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S13" t="n">
+        <v>15000</v>
       </c>
     </row>
     <row r="14">
@@ -1296,24 +1419,33 @@
         </is>
       </c>
       <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
         <v>1108.333333333333</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M14" t="n">
+      <c r="O14" t="n">
         <v>47.3</v>
       </c>
-      <c r="N14" t="n">
+      <c r="P14" t="n">
         <v>52424.16666666667</v>
       </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
+      <c r="Q14" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R14" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S14" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="15">
@@ -1354,24 +1486,33 @@
         </is>
       </c>
       <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
         <v>1108.333333333333</v>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M15" t="n">
+      <c r="O15" t="n">
         <v>47.3</v>
       </c>
-      <c r="N15" t="n">
+      <c r="P15" t="n">
         <v>52424.16666666667</v>
       </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0</v>
+      <c r="Q15" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R15" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S15" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="16">
@@ -1416,24 +1557,33 @@
         </is>
       </c>
       <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>3275</v>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M16" t="n">
+      <c r="O16" t="n">
         <v>70</v>
       </c>
-      <c r="N16" t="n">
+      <c r="P16" t="n">
         <v>229250</v>
       </c>
-      <c r="O16" t="n">
-        <v>36000</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
+      <c r="Q16" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R16" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S16" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="17">
@@ -1478,24 +1628,33 @@
         </is>
       </c>
       <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
         <v>3275</v>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M17" t="n">
+      <c r="O17" t="n">
         <v>70</v>
       </c>
-      <c r="N17" t="n">
+      <c r="P17" t="n">
         <v>229250</v>
       </c>
-      <c r="O17" t="n">
-        <v>180000</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0</v>
+      <c r="Q17" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R17" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S17" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="18">
@@ -1540,24 +1699,33 @@
         </is>
       </c>
       <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
         <v>9432</v>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>5 000 tot 10 000 m²</t>
         </is>
       </c>
-      <c r="M18" t="n">
+      <c r="O18" t="n">
         <v>58.2</v>
       </c>
-      <c r="N18" t="n">
+      <c r="P18" t="n">
         <v>548942.4</v>
       </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
+      <c r="Q18" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R18" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S18" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="19">
@@ -1602,24 +1770,33 @@
         </is>
       </c>
       <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
         <v>8515</v>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>5 000 tot 10 000 m²</t>
         </is>
       </c>
-      <c r="M19" t="n">
+      <c r="O19" t="n">
         <v>173.8</v>
       </c>
-      <c r="N19" t="n">
+      <c r="P19" t="n">
         <v>1479907</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
+      <c r="Q19" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R19" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S19" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="20">
@@ -1664,24 +1841,33 @@
         </is>
       </c>
       <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
         <v>4929</v>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M20" t="n">
+      <c r="O20" t="n">
         <v>139.5</v>
       </c>
-      <c r="N20" t="n">
+      <c r="P20" t="n">
         <v>687595.5</v>
       </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0</v>
+      <c r="Q20" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R20" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S20" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="21">
@@ -1726,24 +1912,33 @@
         </is>
       </c>
       <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
         <v>1378</v>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M21" t="n">
+      <c r="O21" t="n">
         <v>46.9</v>
       </c>
-      <c r="N21" t="n">
+      <c r="P21" t="n">
         <v>64628.2</v>
       </c>
-      <c r="O21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0</v>
+      <c r="Q21" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R21" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S21" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="22">
@@ -1788,24 +1983,33 @@
         </is>
       </c>
       <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
         <v>9457</v>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="N22" t="inlineStr">
         <is>
           <t>5 000 tot 10 000 m²</t>
         </is>
       </c>
-      <c r="M22" t="n">
+      <c r="O22" t="n">
         <v>53.7</v>
       </c>
-      <c r="N22" t="n">
+      <c r="P22" t="n">
         <v>507840.9</v>
       </c>
-      <c r="O22" t="n">
-        <v>540000</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0</v>
+      <c r="Q22" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R22" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S22" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="23">
@@ -1850,24 +2054,33 @@
         </is>
       </c>
       <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
         <v>32522</v>
       </c>
-      <c r="L23" t="inlineStr">
+      <c r="N23" t="inlineStr">
         <is>
           <t>10 000 tot 25 000 m²</t>
         </is>
       </c>
-      <c r="M23" t="n">
+      <c r="O23" t="n">
         <v>69.8</v>
       </c>
-      <c r="N23" t="n">
+      <c r="P23" t="n">
         <v>2270035.6</v>
       </c>
-      <c r="O23" t="n">
-        <v>1080000</v>
-      </c>
-      <c r="P23" t="n">
-        <v>360000</v>
+      <c r="Q23" t="n">
+        <v>137500</v>
+      </c>
+      <c r="R23" t="n">
+        <v>137500</v>
+      </c>
+      <c r="S23" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="24">
@@ -1912,24 +2125,33 @@
         </is>
       </c>
       <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
         <v>1533</v>
       </c>
-      <c r="L24" t="inlineStr">
+      <c r="N24" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M24" t="n">
+      <c r="O24" t="n">
         <v>55.6</v>
       </c>
-      <c r="N24" t="n">
+      <c r="P24" t="n">
         <v>85234.8</v>
       </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
+      <c r="Q24" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R24" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S24" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="25">
@@ -1974,24 +2196,33 @@
         </is>
       </c>
       <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
         <v>2339</v>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="N25" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M25" t="n">
+      <c r="O25" t="n">
         <v>55.6</v>
       </c>
-      <c r="N25" t="n">
+      <c r="P25" t="n">
         <v>130048.4</v>
       </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
+      <c r="Q25" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R25" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S25" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="26">
@@ -2036,24 +2267,33 @@
         </is>
       </c>
       <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
         <v>2136</v>
       </c>
-      <c r="L26" t="inlineStr">
+      <c r="N26" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M26" t="n">
+      <c r="O26" t="n">
         <v>47.3</v>
       </c>
-      <c r="N26" t="n">
+      <c r="P26" t="n">
         <v>101032.8</v>
       </c>
-      <c r="O26" t="n">
-        <v>36000</v>
-      </c>
-      <c r="P26" t="n">
-        <v>135000</v>
+      <c r="Q26" t="n">
+        <v>30000</v>
+      </c>
+      <c r="R26" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S26" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="27">
@@ -2098,24 +2338,33 @@
         </is>
       </c>
       <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
         <v>15646</v>
       </c>
-      <c r="L27" t="inlineStr">
+      <c r="N27" t="inlineStr">
         <is>
           <t>10 000 tot 25 000 m²</t>
         </is>
       </c>
-      <c r="M27" t="n">
+      <c r="O27" t="n">
         <v>74.09999999999999</v>
       </c>
-      <c r="N27" t="n">
+      <c r="P27" t="n">
         <v>1159368.6</v>
       </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>90000</v>
+      <c r="Q27" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R27" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S27" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="28">
@@ -2160,24 +2409,33 @@
         </is>
       </c>
       <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
         <v>4024</v>
       </c>
-      <c r="L28" t="inlineStr">
+      <c r="N28" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M28" t="n">
+      <c r="O28" t="n">
         <v>50</v>
       </c>
-      <c r="N28" t="n">
+      <c r="P28" t="n">
         <v>201200</v>
       </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
+      <c r="Q28" t="n">
+        <v>20000</v>
+      </c>
+      <c r="R28" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S28" t="n">
+        <v>20000</v>
       </c>
     </row>
     <row r="29">
@@ -2222,24 +2480,33 @@
         </is>
       </c>
       <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
         <v>1911</v>
       </c>
-      <c r="L29" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>1 000 tot 2 500 m²</t>
         </is>
       </c>
-      <c r="M29" t="n">
+      <c r="O29" t="n">
         <v>57</v>
       </c>
-      <c r="N29" t="n">
+      <c r="P29" t="n">
         <v>108927</v>
       </c>
-      <c r="O29" t="n">
-        <v>72000</v>
-      </c>
-      <c r="P29" t="n">
-        <v>27000</v>
+      <c r="Q29" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R29" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S29" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="30">
@@ -2262,10 +2529,10 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G30" t="n">
         <v>10</v>
@@ -2284,24 +2551,33 @@
         </is>
       </c>
       <c r="K30" t="n">
+        <v>3</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
         <v>8636</v>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>5 000 tot 10 000 m²</t>
         </is>
       </c>
-      <c r="M30" t="n">
+      <c r="O30" t="n">
         <v>53.7</v>
       </c>
-      <c r="N30" t="n">
+      <c r="P30" t="n">
         <v>237800</v>
       </c>
-      <c r="O30" t="n">
-        <v>360000</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
+      <c r="Q30" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R30" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S30" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="31">
@@ -2346,24 +2622,33 @@
         </is>
       </c>
       <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
         <v>622</v>
       </c>
-      <c r="L31" t="inlineStr">
+      <c r="N31" t="inlineStr">
         <is>
           <t>500 tot 1 000 m²</t>
         </is>
       </c>
-      <c r="M31" t="n">
+      <c r="O31" t="n">
         <v>243.6</v>
       </c>
-      <c r="N31" t="n">
+      <c r="P31" t="n">
         <v>151519.2</v>
       </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
+      <c r="Q31" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R31" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S31" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="32">
@@ -2408,24 +2693,33 @@
         </is>
       </c>
       <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
         <v>3124.75</v>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M32" t="n">
+      <c r="O32" t="n">
         <v>70</v>
       </c>
-      <c r="N32" t="n">
+      <c r="P32" t="n">
         <v>218732.5</v>
       </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
+      <c r="Q32" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R32" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S32" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="33">
@@ -2470,24 +2764,33 @@
         </is>
       </c>
       <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
         <v>3124.75</v>
       </c>
-      <c r="L33" t="inlineStr">
+      <c r="N33" t="inlineStr">
         <is>
           <t>2 500 tot 5 000 m²</t>
         </is>
       </c>
-      <c r="M33" t="n">
+      <c r="O33" t="n">
         <v>50</v>
       </c>
-      <c r="N33" t="n">
+      <c r="P33" t="n">
         <v>156237.5</v>
       </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" t="n">
-        <v>0</v>
+      <c r="Q33" t="n">
+        <v>18000</v>
+      </c>
+      <c r="R33" t="n">
+        <v>54505</v>
+      </c>
+      <c r="S33" t="n">
+        <v>18000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>